<commit_message>
jsut needs a few fixes. still parsing the last of the excel files for issues. Almost perfect :)
</commit_message>
<xml_diff>
--- a/Files/Vaccine_April 14, 2006.xlsx
+++ b/Files/Vaccine_April 14, 2006.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="174">
   <si>
     <t xml:space="preserve">Vaccine</t>
   </si>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">Contract Number</t>
   </si>
   <si>
-    <t xml:space="preserve">DTaP</t>
+    <t xml:space="preserve">DTaP/</t>
   </si>
   <si>
     <t xml:space="preserve">Tripedia</t>
@@ -103,7 +103,7 @@
     <t xml:space="preserve">$70.72</t>
   </si>
   <si>
-    <t xml:space="preserve">DTaP </t>
+    <t xml:space="preserve">DTaP-Hib </t>
   </si>
   <si>
     <t xml:space="preserve">TriHIBit</t>
@@ -139,7 +139,7 @@
     <t xml:space="preserve">$26.34</t>
   </si>
   <si>
-    <t xml:space="preserve">Hepatitis B^</t>
+    <t xml:space="preserve">Hepatitis B-Hib</t>
   </si>
   <si>
     <t xml:space="preserve">COMVAX</t>
@@ -175,7 +175,7 @@
     <t xml:space="preserve">$28.74</t>
   </si>
   <si>
-    <t xml:space="preserve">Hepatitis A-Hepatitis B 18 only^</t>
+    <t xml:space="preserve">Hepatitis A-Hepatitis B 18 only</t>
   </si>
   <si>
     <t xml:space="preserve">Twinrix</t>
@@ -193,13 +193,13 @@
     <t xml:space="preserve">$78.42</t>
   </si>
   <si>
-    <t xml:space="preserve">Hepatitis B PediatricAdolescent</t>
+    <t xml:space="preserve">Hepatitis B Pediatric/Adolescent</t>
   </si>
   <si>
     <t xml:space="preserve">ENGERIX B</t>
   </si>
   <si>
-    <t xml:space="preserve">1 dose vials 10 pack - 1 dose vials 5 pack - 1 dose T-L syringes, No Needle </t>
+    <t xml:space="preserve">1 dose vials </t>
   </si>
   <si>
     <t xml:space="preserve">$9.10</t>
@@ -208,6 +208,12 @@
     <t xml:space="preserve">$21.37</t>
   </si>
   <si>
+    <t xml:space="preserve">10 pack - 1 dose vials </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 pack - 1 dose T-L syringes, No Needle </t>
+  </si>
+  <si>
     <t xml:space="preserve">RECOMBIVAX HB</t>
   </si>
   <si>
@@ -265,16 +271,16 @@
     <t xml:space="preserve">Menactra</t>
   </si>
   <si>
-    <t xml:space="preserve">1 dose vials 5 pack - 1 dose vials </t>
-  </si>
-  <si>
     <t xml:space="preserve">$68.00</t>
   </si>
   <si>
     <t xml:space="preserve">$82.00</t>
   </si>
   <si>
-    <t xml:space="preserve">Measles, Mumps and Rubella ( MMR)</t>
+    <t xml:space="preserve">5 pack - 1 dose vials </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Measles, Mumps and Rubella ( MMR)/</t>
   </si>
   <si>
     <t xml:space="preserve">MMRII</t>
@@ -286,7 +292,7 @@
     <t xml:space="preserve">$40.37</t>
   </si>
   <si>
-    <t xml:space="preserve">Pneumococcal7-valent (Pediatric)</t>
+    <t xml:space="preserve">Pneumococcal 7-valent (Pediatric)</t>
   </si>
   <si>
     <t xml:space="preserve">Prevnar</t>
@@ -319,13 +325,13 @@
     <t xml:space="preserve">$63.25</t>
   </si>
   <si>
-    <t xml:space="preserve">Tetanus  Diphtheria Toxoids^</t>
+    <t xml:space="preserve">Tetanus  Diphtheria Toxoids</t>
   </si>
   <si>
     <t xml:space="preserve">DECAVAC</t>
   </si>
   <si>
-    <t xml:space="preserve">10 pack - 1 dose syringes No Needle 10 pack - 1 dose vials </t>
+    <t xml:space="preserve">10 pack - 1 dose syringes No Needle </t>
   </si>
   <si>
     <t xml:space="preserve">$16.62</t>
@@ -334,21 +340,21 @@
     <t xml:space="preserve">$18.30</t>
   </si>
   <si>
-    <t xml:space="preserve">Tetanus Toxoid, Reduced Diphtheria Toxoid and Acellular Pertussis</t>
+    <t xml:space="preserve">Tetanus Toxoid, Reduced Diphtheria Toxoid and Acellular Pertussis/</t>
   </si>
   <si>
     <t xml:space="preserve">BOOSTRIX</t>
   </si>
   <si>
-    <t xml:space="preserve">10 pack - 1 dose vials 5 pack - 1 dose TL syringes, No Needle </t>
-  </si>
-  <si>
     <t xml:space="preserve">$30.75</t>
   </si>
   <si>
     <t xml:space="preserve">$36.25</t>
   </si>
   <si>
+    <t xml:space="preserve">5 pack - 1 dose TL syringes, No Needle </t>
+  </si>
+  <si>
     <t xml:space="preserve">ADACEL</t>
   </si>
   <si>
@@ -379,33 +385,24 @@
     <t xml:space="preserve">$59.99</t>
   </si>
   <si>
-    <t xml:space="preserve">HepatitisA Adult</t>
-  </si>
-  <si>
     <t xml:space="preserve">$56.17</t>
   </si>
   <si>
     <t xml:space="preserve">$54.98</t>
   </si>
   <si>
-    <t xml:space="preserve">Hepatitis A-Hepatitis B Adult^</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 pack - 1 dose vials 5 pack - 1 dose T-L syringes, No Needle </t>
+    <t xml:space="preserve">Hepatitis A-Hepatitis B Adult</t>
   </si>
   <si>
     <t xml:space="preserve">$36.91</t>
   </si>
   <si>
-    <t xml:space="preserve">HepatitisB-Adult</t>
+    <t xml:space="preserve">Hepatitis B-Adult</t>
   </si>
   <si>
     <t xml:space="preserve">RECOMBIVAX</t>
   </si>
   <si>
-    <t xml:space="preserve">1 dose vials 10 pack - 1 dose vials </t>
-  </si>
-  <si>
     <t xml:space="preserve">$19.36</t>
   </si>
   <si>
@@ -457,7 +454,7 @@
     <t xml:space="preserve">Massachusetts Biologic Labs (Henry Schein Inc.)</t>
   </si>
   <si>
-    <t xml:space="preserve">Influenza  (Age 6 months and older)</t>
+    <t xml:space="preserve">Influenza   (Age 6 months and older)</t>
   </si>
   <si>
     <t xml:space="preserve">Fluzone</t>
@@ -469,7 +466,7 @@
     <t xml:space="preserve">$11.198</t>
   </si>
   <si>
-    <t xml:space="preserve">Influenza (Age 6-35 months)</t>
+    <t xml:space="preserve">Influenza  (Age 6-35 months)</t>
   </si>
   <si>
     <t xml:space="preserve">Fluzone
@@ -485,7 +482,7 @@
     <t xml:space="preserve">$13.613</t>
   </si>
   <si>
-    <t xml:space="preserve">Influenza (Age 36 months and older)</t>
+    <t xml:space="preserve">Influenza  (Age 36 months and older)</t>
   </si>
   <si>
     <t xml:space="preserve">$13.55</t>
@@ -497,7 +494,7 @@
     <t xml:space="preserve">No-Preservative</t>
   </si>
   <si>
-    <t xml:space="preserve">Influenza  (Age 4 years and older)</t>
+    <t xml:space="preserve">Influenza   (Age 4 years and older)</t>
   </si>
   <si>
     <t xml:space="preserve">Fluvirin</t>
@@ -512,7 +509,7 @@
     <t xml:space="preserve">Chiron</t>
   </si>
   <si>
-    <t xml:space="preserve">Influenza (Age 18 years and older)</t>
+    <t xml:space="preserve">Influenza  (Age 18 years and older)</t>
   </si>
   <si>
     <t xml:space="preserve">Fluarix</t>
@@ -524,7 +521,7 @@
     <t xml:space="preserve">$12.00</t>
   </si>
   <si>
-    <t xml:space="preserve">Influenza Live, Intranasal (Age 5-49 years)</t>
+    <t xml:space="preserve">Influenza  Live, Intranasal (Age 5-49 years)</t>
   </si>
   <si>
     <t xml:space="preserve">FluMist</t>
@@ -1201,7 +1198,7 @@
         <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E19" t="s">
         <v>62</v>
@@ -1230,7 +1227,7 @@
         <v>11</v>
       </c>
       <c r="D20" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E20" t="s">
         <v>62</v>
@@ -1253,7 +1250,7 @@
         <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C21" t="s">
         <v>11</v>
@@ -1262,10 +1259,10 @@
         <v>12</v>
       </c>
       <c r="E21" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F21" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G21" s="1">
         <v>39172</v>
@@ -1279,10 +1276,10 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C22" t="s">
         <v>11</v>
@@ -1291,10 +1288,10 @@
         <v>12</v>
       </c>
       <c r="E22" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F22" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G22" s="1">
         <v>39172</v>
@@ -1308,10 +1305,10 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C23" t="s">
         <v>11</v>
@@ -1320,10 +1317,10 @@
         <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F23" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G23" s="1">
         <v>39172</v>
@@ -1337,10 +1334,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C24" t="s">
         <v>11</v>
@@ -1349,10 +1346,10 @@
         <v>31</v>
       </c>
       <c r="E24" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F24" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G24" s="1">
         <v>39172</v>
@@ -1366,10 +1363,10 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C25" t="s">
         <v>11</v>
@@ -1378,10 +1375,10 @@
         <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F25" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G25" s="1">
         <v>39172</v>
@@ -1395,22 +1392,22 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B26" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C26" t="s">
         <v>11</v>
       </c>
       <c r="D26" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="E26" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F26" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G26" s="1">
         <v>39172</v>
@@ -1424,22 +1421,22 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B27" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C27" t="s">
         <v>11</v>
       </c>
       <c r="D27" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E27" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F27" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G27" s="1">
         <v>39172</v>
@@ -1453,10 +1450,10 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B28" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C28" t="s">
         <v>11</v>
@@ -1465,10 +1462,10 @@
         <v>12</v>
       </c>
       <c r="E28" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F28" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G28" s="1">
         <v>39172</v>
@@ -1482,28 +1479,28 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B29" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C29" t="s">
         <v>11</v>
       </c>
       <c r="D29" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E29" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F29" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G29" s="1">
         <v>39172</v>
       </c>
       <c r="H29" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="I29" t="s">
         <v>11</v>
@@ -1511,22 +1508,22 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B30" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C30" t="s">
         <v>11</v>
       </c>
       <c r="D30" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E30" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F30" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G30" s="1">
         <v>39172</v>
@@ -1540,22 +1537,22 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B31" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C31" t="s">
         <v>11</v>
       </c>
       <c r="D31" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E31" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F31" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G31" s="1">
         <v>39172</v>
@@ -1569,22 +1566,22 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B32" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C32" t="s">
         <v>11</v>
       </c>
       <c r="D32" t="s">
-        <v>103</v>
+        <v>64</v>
       </c>
       <c r="E32" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F32" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G32" s="1">
         <v>39172</v>
@@ -1598,22 +1595,22 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B33" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C33" t="s">
         <v>11</v>
       </c>
       <c r="D33" t="s">
-        <v>108</v>
+        <v>64</v>
       </c>
       <c r="E33" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F33" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G33" s="1">
         <v>39172</v>
@@ -1627,22 +1624,22 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B34" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C34" t="s">
         <v>11</v>
       </c>
       <c r="D34" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E34" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F34" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G34" s="1">
         <v>39172</v>
@@ -1656,10 +1653,10 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B35" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C35" t="s">
         <v>11</v>
@@ -1668,10 +1665,10 @@
         <v>12</v>
       </c>
       <c r="E35" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F35" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G35" s="1">
         <v>39172</v>
@@ -1685,10 +1682,10 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B36" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C36" t="s">
         <v>11</v>
@@ -1697,10 +1694,10 @@
         <v>12</v>
       </c>
       <c r="E36" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F36" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G36" s="1">
         <v>39172</v>
@@ -1759,7 +1756,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
         <v>47</v>
@@ -1771,10 +1768,10 @@
         <v>51</v>
       </c>
       <c r="E2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G2" s="1">
         <v>38898</v>
@@ -1788,7 +1785,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s">
         <v>47</v>
@@ -1800,10 +1797,10 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G3" s="1">
         <v>38898</v>
@@ -1817,7 +1814,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s">
         <v>50</v>
@@ -1829,10 +1826,10 @@
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G4" s="1">
         <v>38898</v>
@@ -1846,7 +1843,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
         <v>50</v>
@@ -1858,10 +1855,10 @@
         <v>57</v>
       </c>
       <c r="E5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G5" s="1">
         <v>38898</v>
@@ -1875,7 +1872,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B6" t="s">
         <v>54</v>
@@ -1884,7 +1881,7 @@
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>125</v>
+        <v>64</v>
       </c>
       <c r="E6" t="s">
         <v>126</v>
@@ -1904,7 +1901,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B7" t="s">
         <v>54</v>
@@ -1913,7 +1910,7 @@
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>125</v>
+        <v>65</v>
       </c>
       <c r="E7" t="s">
         <v>126</v>
@@ -1942,13 +1939,13 @@
         <v>11</v>
       </c>
       <c r="D8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" t="s">
         <v>129</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>130</v>
-      </c>
-      <c r="F8" t="s">
-        <v>131</v>
       </c>
       <c r="G8" s="1">
         <v>38898</v>
@@ -1965,19 +1962,19 @@
         <v>127</v>
       </c>
       <c r="B9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" t="s">
         <v>132</v>
       </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>129</v>
-      </c>
-      <c r="E9" t="s">
-        <v>133</v>
-      </c>
       <c r="F9" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G9" s="1">
         <v>38898</v>
@@ -1994,7 +1991,7 @@
         <v>127</v>
       </c>
       <c r="B10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -2003,10 +2000,10 @@
         <v>61</v>
       </c>
       <c r="E10" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G10" s="1">
         <v>38898</v>
@@ -2023,19 +2020,19 @@
         <v>127</v>
       </c>
       <c r="B11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E11" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G11" s="1">
         <v>38898</v>
@@ -2052,19 +2049,19 @@
         <v>127</v>
       </c>
       <c r="B12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E12" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G12" s="1">
         <v>38898</v>
@@ -2078,22 +2075,22 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13" t="s">
         <v>137</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
         <v>138</v>
       </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>139</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>140</v>
-      </c>
-      <c r="F13" t="s">
-        <v>141</v>
       </c>
       <c r="G13" s="1">
         <v>38898</v>
@@ -2107,28 +2104,28 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
         <v>142</v>
       </c>
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>143</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>144</v>
-      </c>
-      <c r="F14" t="s">
-        <v>145</v>
       </c>
       <c r="G14" s="1">
         <v>38898</v>
       </c>
       <c r="H14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I14" t="s">
         <v>11</v>
@@ -2181,10 +2178,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" t="s">
         <v>147</v>
-      </c>
-      <c r="B2" t="s">
-        <v>148</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -2193,10 +2190,10 @@
         <v>36</v>
       </c>
       <c r="E2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F2" t="s">
         <v>149</v>
-      </c>
-      <c r="F2" t="s">
-        <v>150</v>
       </c>
       <c r="G2" s="1">
         <v>39141</v>
@@ -2210,22 +2207,22 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" t="s">
         <v>151</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>152</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>153</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>154</v>
-      </c>
-      <c r="F3" t="s">
-        <v>155</v>
       </c>
       <c r="G3" s="1">
         <v>39141</v>
@@ -2239,22 +2236,22 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E4" t="s">
         <v>156</v>
       </c>
-      <c r="B4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>153</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>157</v>
-      </c>
-      <c r="F4" t="s">
-        <v>158</v>
       </c>
       <c r="G4" s="1">
         <v>39141</v>
@@ -2268,10 +2265,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -2280,10 +2277,10 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F5" t="s">
         <v>157</v>
-      </c>
-      <c r="F5" t="s">
-        <v>158</v>
       </c>
       <c r="G5" s="1">
         <v>39141</v>
@@ -2297,10 +2294,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B6" t="s">
         <v>160</v>
-      </c>
-      <c r="B6" t="s">
-        <v>161</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -2309,16 +2306,16 @@
         <v>36</v>
       </c>
       <c r="E6" t="s">
+        <v>161</v>
+      </c>
+      <c r="F6" t="s">
         <v>162</v>
-      </c>
-      <c r="F6" t="s">
-        <v>163</v>
       </c>
       <c r="G6" s="1">
         <v>39141</v>
       </c>
       <c r="H6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I6" t="s">
         <v>11</v>
@@ -2326,19 +2323,19 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B7" t="s">
         <v>165</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
         <v>166</v>
       </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>167</v>
-      </c>
-      <c r="E7" t="s">
-        <v>168</v>
       </c>
       <c r="F7" t="s">
         <v>20</v>
@@ -2355,28 +2352,28 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B8" t="s">
         <v>169</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
         <v>170</v>
       </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>171</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>172</v>
-      </c>
-      <c r="F8" t="s">
-        <v>173</v>
       </c>
       <c r="G8" s="1">
         <v>39141</v>
       </c>
       <c r="H8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I8" t="s">
         <v>11</v>

</xml_diff>